<commit_message>
some refactoring of main hydro file
</commit_message>
<xml_diff>
--- a/CNM_domain_creation/file_pointers.xlsx
+++ b/CNM_domain_creation/file_pointers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\03125327\github\fc_hydro_kalimantan_2022\CNM_domain_creation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A97AB623-671E-4EA7-817B-3E726A162F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFD059CF-C9B0-479A-AF82-59534C76E425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16125" yWindow="5250" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7815" yWindow="3255" windowWidth="26505" windowHeight="13305" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>